<commit_message>
Progression Agriculture - 3418017359 업데이트
</commit_message>
<xml_diff>
--- a/Data/ferny/Progression Agriculture - 3418017359/Progression Agriculture - 3418017359.xlsx
+++ b/Data/ferny/Progression Agriculture - 3418017359/Progression Agriculture - 3418017359.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Progression Agriculture - 3418017359\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5B4A2A-3BC0-4481-AD87-660F1B3B9AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413E5FAB-BF4D-46B2-865C-D6F4E0DF7395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,8 +32,126 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>bjmi0</author>
+  </authors>
+  <commentList>
+    <comment ref="E30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-09</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>새로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>추가된</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>노드들</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (3</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>개</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="133">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -68,6 +186,18 @@
     <t>DesignationCategoryDef+Ferny_Farming.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>농사</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Ferny_Farming.description</t>
   </si>
   <si>
@@ -77,6 +207,18 @@
     <t>JobDef+UnlockCrop.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>농사와 작물에 관련된 것들입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>JobDef</t>
   </si>
   <si>
@@ -86,6 +228,9 @@
     <t>unlock crop</t>
   </si>
   <si>
+    <t>작물 해금</t>
+  </si>
+  <si>
     <t>JobDef+UnlockCrop.reportString</t>
   </si>
   <si>
@@ -98,6 +243,18 @@
     <t>ThingCategoryDef+SeedBundles.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>{0} 해금 중</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingCategoryDef</t>
   </si>
   <si>
@@ -107,6 +264,9 @@
     <t>seed bundles</t>
   </si>
   <si>
+    <t>씨앗 묶음</t>
+  </si>
+  <si>
     <t>ThingDef+SeedPackingBench.label</t>
   </si>
   <si>
@@ -119,6 +279,9 @@
     <t>Seed packing bench</t>
   </si>
   <si>
+    <t>씨앗 포장 작업대</t>
+  </si>
+  <si>
     <t>ThingDef+SeedPackingBench.description</t>
   </si>
   <si>
@@ -128,6 +291,9 @@
     <t>A workbench for packing seed bundles from harvested crops.</t>
   </si>
   <si>
+    <t>수확한 작물로 씨앗 묶음을 만드는 작업대입니다.</t>
+  </si>
+  <si>
     <t>ThingDef+SeedPackingCraftingSpot.label</t>
   </si>
   <si>
@@ -137,6 +303,9 @@
     <t>Seed packing spot</t>
   </si>
   <si>
+    <t>씨앗 포장 장소</t>
+  </si>
+  <si>
     <t>ThingDef+SeedPackingCraftingSpot.description</t>
   </si>
   <si>
@@ -146,6 +315,9 @@
     <t>A spot for packing seed bundles from harvested crops at double the cost of a traditional packing bench.</t>
   </si>
   <si>
+    <t>일반 포장 작업대보다 두 배의 비용으로 수확한 작물의 씨앗 묶음을 포장하는 장소입니다.</t>
+  </si>
+  <si>
     <t>TraderKindDef+AgriculturalTrader.label</t>
   </si>
   <si>
@@ -161,6 +333,18 @@
     <t>WorkGiverDef+DoBillsPackingSeeds.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>종자 상인</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>WorkGiverDef</t>
   </si>
   <si>
@@ -170,6 +354,9 @@
     <t>make seed bundles</t>
   </si>
   <si>
+    <t>씨앗 묶음 제작</t>
+  </si>
+  <si>
     <t>WorkGiverDef+DoBillsPackingSeeds.verb</t>
   </si>
   <si>
@@ -191,6 +378,18 @@
     <t>Keyed+PA.RecipeLabelMakeSeedBundle</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>에서 씨앗 묶음 제작</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Keyed</t>
   </si>
   <si>
@@ -203,12 +402,48 @@
     <t>Keyed+PA.RecipeDescriptionCraftSeedBundleFrom</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>{0} 씨앗 묶음 제작</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PA.RecipeDescriptionCraftSeedBundleFrom</t>
   </si>
   <si>
     <t>Keyed+PA.RecipeJobStringPackingSeeds</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>Craft a {0} seed bundle from {1} {2}.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>{2} {1}개로 {0} 씨앗 묶음 제작</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PA.RecipeJobStringPackingSeeds</t>
   </si>
   <si>
@@ -218,12 +453,27 @@
     <t>Keyed+PA.SeedBundleLabelSeedBundle</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>{0} 씨앗 포장 중</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PA.SeedBundleLabelSeedBundle</t>
   </si>
   <si>
     <t>{0} seed bundle</t>
   </si>
   <si>
+    <t>{0} 씨앗 묶음</t>
+  </si>
+  <si>
     <t>Keyed+PA.SeedBundleDescriptionBundleOfSeedsForCrop</t>
   </si>
   <si>
@@ -236,6 +486,18 @@
     <t>Keyed+PA.CropUnlocked</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>{0} 씨앗 묶음입니다. 이 묶음을 열어 해당 작물을 재배할 수 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PA.CropUnlocked</t>
   </si>
   <si>
@@ -245,6 +507,18 @@
     <t>Keyed+PA.CropUnlockedDesc</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>{0} 씨앗 발견!</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PA.CropUnlockedDesc</t>
   </si>
   <si>
@@ -254,12 +528,27 @@
     <t>Keyed+PA.UnlockCrop</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>씨앗 묶음을 열어 {0} 씨앗을 가득 획득했습니다! 이제 {0}(을)를 재배할 수 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PA.UnlockCrop</t>
   </si>
   <si>
     <t>Open {0} seed bundle</t>
   </si>
   <si>
+    <t>{0} 씨앗 묶음 열기</t>
+  </si>
+  <si>
     <t>Keyed+PA.CropAlreadyUnlocked</t>
   </si>
   <si>
@@ -272,6 +561,18 @@
     <t>Keyed+PA.SeedBundleIngredientCount</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>{0}(이)가 해금됨</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PA.SeedBundleIngredientCount</t>
   </si>
   <si>
@@ -281,6 +582,18 @@
     <t>Keyed+PA.CropIsNotUnlocked</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>씨앗 묶음 재료 수량: {0}</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PA.CropIsNotUnlocked</t>
   </si>
   <si>
@@ -290,6 +603,18 @@
     <t>Keyed+PA.YouUnlockedSeed</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>{0}(이)가 아직 해금되지 않음</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PA.YouUnlockedSeed</t>
   </si>
   <si>
@@ -299,6 +624,18 @@
     <t>Keyed+PA.NothingToSowYet</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>이미 획득한 묶음입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PA.NothingToSowYet</t>
   </si>
   <si>
@@ -308,108 +645,77 @@
     <t>Keyed+PA.UnlockNewSeeds</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>파종 중인 작물이 없습니다. 클릭하여 메뉴를 여세요.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>PA.UnlockNewSeeds</t>
   </si>
   <si>
     <t>Open seed bundles in order to be able to sow plants. These can be found trading, raiding, or through quest rewards.</t>
   </si>
   <si>
-    <t>작물 해금</t>
-  </si>
-  <si>
-    <t>씨앗 묶음</t>
-  </si>
-  <si>
-    <t>씨앗 포장 작업대</t>
-  </si>
-  <si>
-    <t>수확한 작물로 씨앗 묶음을 만드는 작업대입니다.</t>
-  </si>
-  <si>
-    <t>씨앗 포장 장소</t>
-  </si>
-  <si>
-    <t>일반 포장 작업대보다 두 배의 비용으로 수확한 작물의 씨앗 묶음을 포장하는 장소입니다.</t>
-  </si>
-  <si>
-    <t>씨앗 묶음 제작</t>
-  </si>
-  <si>
-    <t>{0} 씨앗 묶음</t>
-  </si>
-  <si>
-    <t>{0} 씨앗 묶음 열기</t>
-  </si>
-  <si>
-    <t>농사</t>
+    <t>ScenPartDef+Ferny_StartingSeeds.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>식물을 심으려면 씨앗 묶음을 열어야 합니다. 씨앗 묶음은 거래, 습격, 임무 보상 등으로 얻을 수 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ScenPartDef</t>
+  </si>
+  <si>
+    <t>Ferny_StartingSeeds.label</t>
+  </si>
+  <si>
+    <t>Start with seed bundle</t>
+  </si>
+  <si>
+    <t>Keyed+PA.UnlockedSeedLabel</t>
+  </si>
+  <si>
+    <t>Keyed+PA.ScenPart_StartingSeeds</t>
+  </si>
+  <si>
+    <t>PA.ScenPart_StartingSeeds</t>
+  </si>
+  <si>
+    <t>씨앗 묶음과 함께 시작</t>
+  </si>
+  <si>
+    <t>Start with seed bundle</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>농사와 작물에 관련된 것들입니다.</t>
+    <t>씨앗 묶음과 함께 시작</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>{0} 해금 중</t>
+    <t>{0} (owned)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>종자 상인</t>
+    <t>PA.UnlockedSeedLabel</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>에서 씨앗 묶음 제작</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0} 씨앗 묶음 제작</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0} 씨앗 포장 중</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Craft a {0} seed bundle from {1} {2}.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{2} {1}개로 {0} 씨앗 묶음 제작</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0} 씨앗 묶음입니다. 이 묶음을 열어 해당 작물을 재배할 수 있습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0} 씨앗 발견!</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>씨앗 묶음을 열어 {0} 씨앗을 가득 획득했습니다! 이제 {0}(을)를 재배할 수 있습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이미 획득한 묶음입니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0}(이)가 아직 해금되지 않음</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0}(이)가 해금됨</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>씨앗 묶음 재료 수량: {0}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>파종 중인 작물이 없습니다. 클릭하여 메뉴를 여세요.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>식물을 심으려면 씨앗 묶음을 열어야 합니다. 씨앗 묶음은 거래, 습격, 임무 보상 등으로 얻을 수 있습니다.</t>
+    <t>{0} (획득 완료)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -417,7 +723,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -436,13 +742,31 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -457,9 +781,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -761,17 +1086,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="7" width="9.1796875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -808,7 +1133,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -819,442 +1144,494 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>104</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
         <v>119</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>